<commit_message>
add dataset05 no tail cropping ROIs and crop table
</commit_message>
<xml_diff>
--- a/dataset05-cropping-table-babb02.1,babb03-no_tail.xlsx
+++ b/dataset05-cropping-table-babb02.1,babb03-no_tail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83ED852-CE47-497F-957C-AFE2070601A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9651883-DA2A-4E58-A731-D3B2F82091C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>488 nm</t>
+  </si>
+  <si>
+    <t>belly toward high z value</t>
+  </si>
+  <si>
+    <t>belly toward high x value</t>
+  </si>
+  <si>
+    <t>belly toward high y value</t>
   </si>
 </sst>
 </file>
@@ -508,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -521,11 +530,11 @@
     <col min="3" max="8" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="9.7109375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="9.140625" collapsed="1"/>
-    <col min="21" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -586,14 +595,41 @@
       <c r="T1" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="J2">
+        <v>345</v>
+      </c>
+      <c r="K2">
+        <v>643</v>
+      </c>
+      <c r="M2">
+        <v>313</v>
+      </c>
+      <c r="N2">
+        <v>923</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+      <c r="Q2">
+        <v>92</v>
+      </c>
       <c r="R2">
         <v>995</v>
       </c>
@@ -603,14 +639,41 @@
       <c r="T2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J3">
+        <v>587</v>
+      </c>
+      <c r="K3">
+        <v>855</v>
+      </c>
+      <c r="M3">
+        <v>237</v>
+      </c>
+      <c r="N3">
+        <v>897</v>
+      </c>
+      <c r="P3">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>92</v>
+      </c>
       <c r="R3">
         <v>995</v>
       </c>
@@ -620,14 +683,41 @@
       <c r="T3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J4">
+        <v>338</v>
+      </c>
+      <c r="K4">
+        <v>642</v>
+      </c>
+      <c r="M4">
+        <v>217</v>
+      </c>
+      <c r="N4">
+        <v>898</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>96</v>
+      </c>
       <c r="R4">
         <v>995</v>
       </c>
@@ -637,14 +727,41 @@
       <c r="T4">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>-1</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="J5">
+        <v>335</v>
+      </c>
+      <c r="K5">
+        <v>662</v>
+      </c>
+      <c r="M5">
+        <v>345</v>
+      </c>
+      <c r="N5">
+        <v>991</v>
+      </c>
+      <c r="P5">
+        <v>9</v>
+      </c>
+      <c r="Q5">
+        <v>97</v>
+      </c>
       <c r="R5">
         <v>995</v>
       </c>
@@ -654,14 +771,41 @@
       <c r="T5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="J6">
+        <v>384</v>
+      </c>
+      <c r="K6">
+        <v>709</v>
+      </c>
+      <c r="M6">
+        <v>327</v>
+      </c>
+      <c r="N6">
+        <v>983</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>97</v>
+      </c>
       <c r="R6">
         <v>995</v>
       </c>
@@ -671,14 +815,41 @@
       <c r="T6">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>-1</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J7">
+        <v>270</v>
+      </c>
+      <c r="K7">
+        <v>624</v>
+      </c>
+      <c r="M7">
+        <v>175</v>
+      </c>
+      <c r="N7">
+        <v>817</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>91</v>
+      </c>
       <c r="R7">
         <v>995</v>
       </c>
@@ -688,14 +859,41 @@
       <c r="T7">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>-1</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="J8">
+        <v>442</v>
+      </c>
+      <c r="K8">
+        <v>878</v>
+      </c>
+      <c r="M8">
+        <v>1090</v>
+      </c>
+      <c r="N8">
+        <v>1914</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>47</v>
+      </c>
       <c r="R8">
         <v>1170</v>
       </c>
@@ -705,14 +903,41 @@
       <c r="T8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>-1</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="J9">
+        <v>503</v>
+      </c>
+      <c r="K9">
+        <v>970</v>
+      </c>
+      <c r="M9">
+        <v>1152</v>
+      </c>
+      <c r="N9">
+        <v>1936</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>55</v>
+      </c>
       <c r="R9">
         <v>1170</v>
       </c>
@@ -722,14 +947,41 @@
       <c r="T9">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>-1</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="J10">
+        <v>387</v>
+      </c>
+      <c r="K10">
+        <v>836</v>
+      </c>
+      <c r="M10">
+        <v>1108</v>
+      </c>
+      <c r="N10">
+        <v>1905</v>
+      </c>
+      <c r="P10">
+        <v>12</v>
+      </c>
+      <c r="Q10">
+        <v>55</v>
+      </c>
       <c r="R10">
         <v>1170</v>
       </c>
@@ -739,14 +991,41 @@
       <c r="T10">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="J11">
+        <v>457</v>
+      </c>
+      <c r="K11">
+        <v>857</v>
+      </c>
+      <c r="M11">
+        <v>1134</v>
+      </c>
+      <c r="N11">
+        <v>1881</v>
+      </c>
+      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <v>60</v>
+      </c>
       <c r="R11">
         <v>1170</v>
       </c>
@@ -756,14 +1035,41 @@
       <c r="T11">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="J12">
+        <v>404</v>
+      </c>
+      <c r="K12">
+        <v>832</v>
+      </c>
+      <c r="M12">
+        <v>1141</v>
+      </c>
+      <c r="N12">
+        <v>1929</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>49</v>
+      </c>
       <c r="R12">
         <v>1170</v>
       </c>
@@ -773,14 +1079,41 @@
       <c r="T12">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>-1</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J13">
+        <v>524</v>
+      </c>
+      <c r="K13">
+        <v>934</v>
+      </c>
+      <c r="M13">
+        <v>976</v>
+      </c>
+      <c r="N13">
+        <v>1878</v>
+      </c>
+      <c r="P13">
+        <v>3</v>
+      </c>
+      <c r="Q13">
+        <v>50</v>
+      </c>
       <c r="R13">
         <v>1170</v>
       </c>
@@ -790,14 +1123,41 @@
       <c r="T13">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="J14">
+        <v>372</v>
+      </c>
+      <c r="K14">
+        <v>774</v>
+      </c>
+      <c r="M14">
+        <v>1127</v>
+      </c>
+      <c r="N14">
+        <v>1918</v>
+      </c>
+      <c r="P14">
+        <v>8</v>
+      </c>
+      <c r="Q14">
+        <v>65</v>
+      </c>
       <c r="R14">
         <v>1170</v>
       </c>
@@ -806,6 +1166,15 @@
       </c>
       <c r="T14">
         <v>65</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>-1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make some calculations; also, finish comprehensive cropping flow chart on paper
</commit_message>
<xml_diff>
--- a/dataset05-cropping-table-babb02.1,babb03-no_tail.xlsx
+++ b/dataset05-cropping-table-babb02.1,babb03-no_tail.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9651883-DA2A-4E58-A731-D3B2F82091C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7946F9A-FC67-4639-905F-7CE5179DA1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -136,6 +147,9 @@
   </si>
   <si>
     <t>belly toward high y value</t>
+  </si>
+  <si>
+    <t>dz ind</t>
   </si>
 </sst>
 </file>
@@ -517,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -530,11 +544,11 @@
     <col min="3" max="8" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="9.7109375" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="9.140625" collapsed="1"/>
-    <col min="21" max="21" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -587,25 +601,28 @@
         <v>28</v>
       </c>
       <c r="R1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -618,38 +635,46 @@
       <c r="K2">
         <v>643</v>
       </c>
+      <c r="L2">
+        <f>K2-J2</f>
+        <v>298</v>
+      </c>
       <c r="M2">
         <v>313</v>
       </c>
       <c r="N2">
         <v>923</v>
       </c>
+      <c r="O2">
+        <f>N2-M2</f>
+        <v>610</v>
+      </c>
       <c r="P2">
         <v>6</v>
       </c>
       <c r="Q2">
         <v>92</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>995</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1699</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>100</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>1</v>
       </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
       <c r="W2">
         <v>0</v>
       </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -662,38 +687,46 @@
       <c r="K3">
         <v>855</v>
       </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L14" si="0">K3-J3</f>
+        <v>268</v>
+      </c>
       <c r="M3">
         <v>237</v>
       </c>
       <c r="N3">
         <v>897</v>
       </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O14" si="1">N3-M3</f>
+        <v>660</v>
+      </c>
       <c r="P3">
         <v>6</v>
       </c>
       <c r="Q3">
         <v>92</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>995</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>1699</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>100</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>1</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
       <c r="W3">
         <v>0</v>
       </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -706,38 +739,46 @@
       <c r="K4">
         <v>642</v>
       </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>304</v>
+      </c>
       <c r="M4">
         <v>217</v>
       </c>
       <c r="N4">
         <v>898</v>
       </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>681</v>
+      </c>
       <c r="P4">
         <v>6</v>
       </c>
       <c r="Q4">
         <v>96</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>995</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>1699</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>105</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>-1</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
       <c r="W4">
         <v>0</v>
       </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -750,38 +791,46 @@
       <c r="K5">
         <v>662</v>
       </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>327</v>
+      </c>
       <c r="M5">
         <v>345</v>
       </c>
       <c r="N5">
         <v>991</v>
       </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>646</v>
+      </c>
       <c r="P5">
         <v>9</v>
       </c>
       <c r="Q5">
         <v>97</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>995</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>1699</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>100</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>1</v>
       </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
       <c r="W5">
         <v>0</v>
       </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -794,38 +843,46 @@
       <c r="K6">
         <v>709</v>
       </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
       <c r="M6">
         <v>327</v>
       </c>
       <c r="N6">
         <v>983</v>
       </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>656</v>
+      </c>
       <c r="P6">
         <v>3</v>
       </c>
       <c r="Q6">
         <v>97</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>995</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>1699</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>97</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>-1</v>
       </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
       <c r="W6">
         <v>0</v>
       </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -838,38 +895,46 @@
       <c r="K7">
         <v>624</v>
       </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>354</v>
+      </c>
       <c r="M7">
         <v>175</v>
       </c>
       <c r="N7">
         <v>817</v>
       </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>642</v>
+      </c>
       <c r="P7">
         <v>5</v>
       </c>
       <c r="Q7">
         <v>91</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>995</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>1699</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>91</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>-1</v>
       </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
       <c r="W7">
         <v>0</v>
       </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -882,38 +947,46 @@
       <c r="K8">
         <v>878</v>
       </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>436</v>
+      </c>
       <c r="M8">
         <v>1090</v>
       </c>
       <c r="N8">
         <v>1914</v>
       </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>824</v>
+      </c>
       <c r="P8">
         <v>4</v>
       </c>
       <c r="Q8">
         <v>47</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>1170</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>1999</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>50</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>-1</v>
       </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
       <c r="W8">
         <v>0</v>
       </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -926,38 +999,46 @@
       <c r="K9">
         <v>970</v>
       </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>467</v>
+      </c>
       <c r="M9">
         <v>1152</v>
       </c>
       <c r="N9">
         <v>1936</v>
       </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>784</v>
+      </c>
       <c r="P9">
         <v>10</v>
       </c>
       <c r="Q9">
         <v>55</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1170</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>1999</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>55</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
       <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>-1</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -970,38 +1051,46 @@
       <c r="K10">
         <v>836</v>
       </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>449</v>
+      </c>
       <c r="M10">
         <v>1108</v>
       </c>
       <c r="N10">
         <v>1905</v>
       </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>797</v>
+      </c>
       <c r="P10">
         <v>12</v>
       </c>
       <c r="Q10">
         <v>55</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>1170</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>1999</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>55</v>
       </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
       <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>1</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1014,38 +1103,46 @@
       <c r="K11">
         <v>857</v>
       </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
       <c r="M11">
         <v>1134</v>
       </c>
       <c r="N11">
         <v>1881</v>
       </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>747</v>
+      </c>
       <c r="P11">
         <v>7</v>
       </c>
       <c r="Q11">
         <v>60</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>1170</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>1999</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>60</v>
       </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
       <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
         <v>1</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1058,38 +1155,46 @@
       <c r="K12">
         <v>832</v>
       </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>428</v>
+      </c>
       <c r="M12">
         <v>1141</v>
       </c>
       <c r="N12">
         <v>1929</v>
       </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>788</v>
+      </c>
       <c r="P12">
         <v>3</v>
       </c>
       <c r="Q12">
         <v>49</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1170</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>1999</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>50</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
       <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <v>-1</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1102,38 +1207,46 @@
       <c r="K13">
         <v>934</v>
       </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
       <c r="M13">
         <v>976</v>
       </c>
       <c r="N13">
         <v>1878</v>
       </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>902</v>
+      </c>
       <c r="P13">
         <v>3</v>
       </c>
       <c r="Q13">
         <v>50</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>1170</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>1999</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>50</v>
       </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
       <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>1</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1146,34 +1259,42 @@
       <c r="K14">
         <v>774</v>
       </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>402</v>
+      </c>
       <c r="M14">
         <v>1127</v>
       </c>
       <c r="N14">
         <v>1918</v>
       </c>
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>791</v>
+      </c>
       <c r="P14">
         <v>8</v>
       </c>
       <c r="Q14">
         <v>65</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1170</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>1999</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>65</v>
       </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
       <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
         <v>-1</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cropping coordinates calculate for dataset05, with my py pandas script
</commit_message>
<xml_diff>
--- a/dataset05-cropping-table-babb02.1,babb03-no_tail.xlsx
+++ b/dataset05-cropping-table-babb02.1,babb03-no_tail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480797D7-A289-4293-8640-5571A10C623C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6D4B14-39B4-4516-8E5D-999E7F51649D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -44,15 +44,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>X (width)</t>
-  </si>
-  <si>
-    <t>Y (height)</t>
-  </si>
-  <si>
-    <t>Z (depth)</t>
-  </si>
-  <si>
     <t>channel used in making this cropping table</t>
   </si>
   <si>
@@ -134,15 +125,6 @@
     <t>dz_ind</t>
   </si>
   <si>
-    <t>z_interest (coordinate)</t>
-  </si>
-  <si>
-    <t>z1_ind (coordinate)</t>
-  </si>
-  <si>
-    <t>z0_ind (coordinate)</t>
-  </si>
-  <si>
     <t>comments_all_rows</t>
   </si>
   <si>
@@ -150,6 +132,24 @@
   </si>
   <si>
     <t>dataset05</t>
+  </si>
+  <si>
+    <t>z_interest</t>
+  </si>
+  <si>
+    <t>x_size</t>
+  </si>
+  <si>
+    <t>y_size</t>
+  </si>
+  <si>
+    <t>z_size</t>
+  </si>
+  <si>
+    <t>z1_ind</t>
+  </si>
+  <si>
+    <t>z0_ind</t>
   </si>
 </sst>
 </file>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,94 +563,94 @@
   <sheetData>
     <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="AB1" s="3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AE1" s="3" t="s">
         <v>31</v>
@@ -658,23 +658,23 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -685,29 +685,17 @@
       <c r="R2">
         <v>643</v>
       </c>
-      <c r="S2">
-        <f>R2-Q2</f>
-        <v>298</v>
-      </c>
       <c r="T2">
         <v>313</v>
       </c>
       <c r="U2">
         <v>923</v>
       </c>
-      <c r="V2">
-        <f>U2-T2</f>
-        <v>610</v>
-      </c>
       <c r="W2">
         <v>5</v>
       </c>
       <c r="X2">
         <v>91</v>
-      </c>
-      <c r="Y2">
-        <f>X2-W2</f>
-        <v>86</v>
       </c>
       <c r="Z2">
         <v>995</v>
@@ -730,23 +718,23 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -757,29 +745,17 @@
       <c r="R3">
         <v>855</v>
       </c>
-      <c r="S3">
-        <f>R3-Q3</f>
-        <v>268</v>
-      </c>
       <c r="T3">
         <v>237</v>
       </c>
       <c r="U3">
         <v>897</v>
       </c>
-      <c r="V3">
-        <f>U3-T3</f>
-        <v>660</v>
-      </c>
       <c r="W3">
         <v>5</v>
       </c>
       <c r="X3">
         <v>91</v>
-      </c>
-      <c r="Y3">
-        <f>X3-W3</f>
-        <v>86</v>
       </c>
       <c r="Z3">
         <v>995</v>
@@ -802,23 +778,23 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B4" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <v>3</v>
@@ -829,29 +805,17 @@
       <c r="R4">
         <v>642</v>
       </c>
-      <c r="S4">
-        <f>R4-Q4</f>
-        <v>304</v>
-      </c>
       <c r="T4">
         <v>217</v>
       </c>
       <c r="U4">
         <v>898</v>
       </c>
-      <c r="V4">
-        <f>U4-T4</f>
-        <v>681</v>
-      </c>
       <c r="W4">
         <v>5</v>
       </c>
       <c r="X4">
         <v>95</v>
-      </c>
-      <c r="Y4">
-        <f>X4-W4</f>
-        <v>90</v>
       </c>
       <c r="Z4">
         <v>995</v>
@@ -874,23 +838,23 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
         <v>4</v>
@@ -901,29 +865,17 @@
       <c r="R5">
         <v>662</v>
       </c>
-      <c r="S5">
-        <f>R5-Q5</f>
-        <v>327</v>
-      </c>
       <c r="T5">
         <v>345</v>
       </c>
       <c r="U5">
         <v>991</v>
       </c>
-      <c r="V5">
-        <f>U5-T5</f>
-        <v>646</v>
-      </c>
       <c r="W5">
         <v>8</v>
       </c>
       <c r="X5">
         <v>96</v>
-      </c>
-      <c r="Y5">
-        <f>X5-W5</f>
-        <v>88</v>
       </c>
       <c r="Z5">
         <v>995</v>
@@ -946,23 +898,23 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B6" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1">
         <v>5</v>
@@ -973,29 +925,17 @@
       <c r="R6">
         <v>709</v>
       </c>
-      <c r="S6">
-        <f>R6-Q6</f>
-        <v>325</v>
-      </c>
       <c r="T6">
         <v>327</v>
       </c>
       <c r="U6">
         <v>983</v>
       </c>
-      <c r="V6">
-        <f>U6-T6</f>
-        <v>656</v>
-      </c>
       <c r="W6">
         <v>2</v>
       </c>
       <c r="X6">
         <v>96</v>
-      </c>
-      <c r="Y6">
-        <f>X6-W6</f>
-        <v>94</v>
       </c>
       <c r="Z6">
         <v>995</v>
@@ -1018,23 +958,23 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B7" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1">
         <v>6</v>
@@ -1045,29 +985,17 @@
       <c r="R7">
         <v>624</v>
       </c>
-      <c r="S7">
-        <f>R7-Q7</f>
-        <v>354</v>
-      </c>
       <c r="T7">
         <v>175</v>
       </c>
       <c r="U7">
         <v>817</v>
       </c>
-      <c r="V7">
-        <f>U7-T7</f>
-        <v>642</v>
-      </c>
       <c r="W7">
         <v>4</v>
       </c>
       <c r="X7">
         <v>90</v>
-      </c>
-      <c r="Y7">
-        <f>X7-W7</f>
-        <v>86</v>
       </c>
       <c r="Z7">
         <v>995</v>
@@ -1090,23 +1018,23 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -1117,29 +1045,17 @@
       <c r="R8">
         <v>878</v>
       </c>
-      <c r="S8">
-        <f>R8-Q8</f>
-        <v>436</v>
-      </c>
       <c r="T8">
         <v>1090</v>
       </c>
       <c r="U8">
         <v>1914</v>
       </c>
-      <c r="V8">
-        <f>U8-T8</f>
-        <v>824</v>
-      </c>
       <c r="W8">
         <v>3</v>
       </c>
       <c r="X8">
         <v>46</v>
-      </c>
-      <c r="Y8">
-        <f>X8-W8</f>
-        <v>43</v>
       </c>
       <c r="Z8">
         <v>1170</v>
@@ -1162,23 +1078,23 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B9" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
@@ -1189,29 +1105,17 @@
       <c r="R9">
         <v>970</v>
       </c>
-      <c r="S9">
-        <f>R9-Q9</f>
-        <v>467</v>
-      </c>
       <c r="T9">
         <v>1152</v>
       </c>
       <c r="U9">
         <v>1936</v>
       </c>
-      <c r="V9">
-        <f>U9-T9</f>
-        <v>784</v>
-      </c>
       <c r="W9">
         <v>9</v>
       </c>
       <c r="X9">
         <v>54</v>
-      </c>
-      <c r="Y9">
-        <f>X9-W9</f>
-        <v>45</v>
       </c>
       <c r="Z9">
         <v>1170</v>
@@ -1234,23 +1138,23 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B10" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -1261,29 +1165,17 @@
       <c r="R10">
         <v>836</v>
       </c>
-      <c r="S10">
-        <f>R10-Q10</f>
-        <v>449</v>
-      </c>
       <c r="T10">
         <v>1108</v>
       </c>
       <c r="U10">
         <v>1905</v>
       </c>
-      <c r="V10">
-        <f>U10-T10</f>
-        <v>797</v>
-      </c>
       <c r="W10">
         <v>11</v>
       </c>
       <c r="X10">
         <v>54</v>
-      </c>
-      <c r="Y10">
-        <f>X10-W10</f>
-        <v>43</v>
       </c>
       <c r="Z10">
         <v>1170</v>
@@ -1306,23 +1198,23 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B11" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1">
         <v>4</v>
@@ -1333,29 +1225,17 @@
       <c r="R11">
         <v>857</v>
       </c>
-      <c r="S11">
-        <f>R11-Q11</f>
-        <v>400</v>
-      </c>
       <c r="T11">
         <v>1134</v>
       </c>
       <c r="U11">
         <v>1881</v>
       </c>
-      <c r="V11">
-        <f>U11-T11</f>
-        <v>747</v>
-      </c>
       <c r="W11">
         <v>6</v>
       </c>
       <c r="X11">
         <v>59</v>
-      </c>
-      <c r="Y11">
-        <f>X11-W11</f>
-        <v>53</v>
       </c>
       <c r="Z11">
         <v>1170</v>
@@ -1378,23 +1258,23 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G12" s="1">
         <v>5</v>
@@ -1405,29 +1285,17 @@
       <c r="R12">
         <v>832</v>
       </c>
-      <c r="S12">
-        <f>R12-Q12</f>
-        <v>428</v>
-      </c>
       <c r="T12">
         <v>1141</v>
       </c>
       <c r="U12">
         <v>1929</v>
       </c>
-      <c r="V12">
-        <f>U12-T12</f>
-        <v>788</v>
-      </c>
       <c r="W12">
         <v>2</v>
       </c>
       <c r="X12">
         <v>48</v>
-      </c>
-      <c r="Y12">
-        <f>X12-W12</f>
-        <v>46</v>
       </c>
       <c r="Z12">
         <v>1170</v>
@@ -1450,23 +1318,23 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B13" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1">
         <v>6</v>
@@ -1477,29 +1345,17 @@
       <c r="R13">
         <v>934</v>
       </c>
-      <c r="S13">
-        <f>R13-Q13</f>
-        <v>410</v>
-      </c>
       <c r="T13">
         <v>976</v>
       </c>
       <c r="U13">
         <v>1878</v>
       </c>
-      <c r="V13">
-        <f>U13-T13</f>
-        <v>902</v>
-      </c>
       <c r="W13">
         <v>2</v>
       </c>
       <c r="X13">
         <v>49</v>
-      </c>
-      <c r="Y13">
-        <f>X13-W13</f>
-        <v>47</v>
       </c>
       <c r="Z13">
         <v>1170</v>
@@ -1522,23 +1378,23 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B14" t="str">
         <f>[1]Tabelle1!B2</f>
         <v>other comments: 1.) x, y, and z values are given as coordinates (counting starts with 0), whereas when duplicating a z-stack in Fiji, the stack number has to be given (where counting starts with 1). 2.) scaled to voxel size of 2.53,2.53,10.</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G14" s="1">
         <v>7</v>
@@ -1549,29 +1405,17 @@
       <c r="R14">
         <v>774</v>
       </c>
-      <c r="S14">
-        <f>R14-Q14</f>
-        <v>402</v>
-      </c>
       <c r="T14">
         <v>1127</v>
       </c>
       <c r="U14">
         <v>1918</v>
       </c>
-      <c r="V14">
-        <f>U14-T14</f>
-        <v>791</v>
-      </c>
       <c r="W14">
         <v>7</v>
       </c>
       <c r="X14">
         <v>64</v>
-      </c>
-      <c r="Y14">
-        <f>X14-W14</f>
-        <v>57</v>
       </c>
       <c r="Z14">
         <v>1170</v>

</xml_diff>